<commit_message>
Update getSeconds to add resolution even if  HR clock rolls over
</commit_message>
<xml_diff>
--- a/Adapter/High Resolution Timing Math.xlsx
+++ b/Adapter/High Resolution Timing Math.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrackAction\GITdevelop\Adapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4C90E6-B834-4FC5-AE5E-1064BE796CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD015AE-42B1-4ECB-AF18-AE0637005D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18210" yWindow="0" windowWidth="27420" windowHeight="17580" xr2:uid="{8B50EA65-C387-4F3F-AF97-6B34053CCFA8}"/>
+    <workbookView xWindow="34935" yWindow="0" windowWidth="16845" windowHeight="34200" xr2:uid="{8B50EA65-C387-4F3F-AF97-6B34053CCFA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,9 +222,9 @@
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="188" formatCode="0.0000000000"/>
-    <numFmt numFmtId="190" formatCode="0.000000000000"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -290,7 +290,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -298,10 +298,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="188" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8307C1F8-92F4-45C5-842D-95C1CA3F53CB}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +784,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="11">
-        <v>4.0010000059999999</v>
+        <v>5.3453429999999997</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -808,7 +808,7 @@
       </c>
       <c r="C18" s="1">
         <f>Ts_LR+FLOOR(ExpectedOutputS*LowResHz,1)</f>
-        <v>5024</v>
+        <v>6368</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="5" t="s">
@@ -828,7 +828,7 @@
       </c>
       <c r="C19" s="1">
         <f>MOD(Ts_HR+(ExpectedOutputS*HighResHz),MaxCycle)</f>
-        <v>2400600002.6000004</v>
+        <v>3207205799</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="5" t="s">
@@ -846,7 +846,7 @@
       </c>
       <c r="C23" s="1">
         <f>Te_LR-Ts_LR</f>
-        <v>4001</v>
+        <v>5345</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="5" t="s">
@@ -859,7 +859,7 @@
       </c>
       <c r="C24" s="4">
         <f>Duration_LR/LowResHz</f>
-        <v>4.0010000000000003</v>
+        <v>5.3449999999999998</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="5" t="s">
@@ -901,7 +901,7 @@
       </c>
       <c r="C29" s="1">
         <f>RollOverHRTicks_Calc+Te_HR-Ts_HR</f>
-        <v>-1894367291.3999996</v>
+        <v>-1087761495</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>10</v>
@@ -913,7 +913,7 @@
       </c>
       <c r="C30" s="1">
         <f>MOD(DurationHRTicks,HighResTicksPerLowResTick)</f>
-        <v>432708.60000038147</v>
+        <v>38505</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>10</v>
@@ -925,7 +925,7 @@
       </c>
       <c r="C31" s="4">
         <f>HighResFractionHRTicks/HighResHz</f>
-        <v>7.2118100000063577E-4</v>
+        <v>6.4175000000000001E-5</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>11</v>
@@ -937,7 +937,7 @@
       </c>
       <c r="C32" s="4">
         <f>C31+C24</f>
-        <v>4.0017211810000006</v>
+        <v>5.3450641750000001</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -968,7 +968,7 @@
       </c>
       <c r="C36" s="1">
         <f>IF(Ts_HR &lt;Te_HR, Te_HR - Ts_HR, Te_HR - ( MaxCycle - Ts_HR))</f>
-        <v>2400600001.6000004</v>
+        <v>3207205798</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>10</v>
@@ -980,7 +980,7 @@
       </c>
       <c r="C37" s="1">
         <f>MOD(C35+C36, HighResTicksPerLowResTick)</f>
-        <v>1.6000003814697266</v>
+        <v>205798</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>10</v>
@@ -992,7 +992,7 @@
       </c>
       <c r="C38" s="4">
         <f>C37/HighResHz</f>
-        <v>2.6666673024495442E-9</v>
+        <v>3.4299666666666668E-4</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>11</v>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="C39" s="8">
         <f>C24+C38</f>
-        <v>4.0010000026666672</v>
+        <v>5.3453429966666661</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>11</v>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="C43" s="1">
         <f>IF(Ts_HR &lt;Te_HR, Te_HR - Ts_HR, Te_HR - ( MaxCycle - Ts_HR))</f>
-        <v>2400600001.6000004</v>
+        <v>3207205798</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>10</v>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="C44" s="1">
         <f>MOD(C42+C43, HighResTicksPerLowResTick)</f>
-        <v>1.6000003814697266</v>
+        <v>205798</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>10</v>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="C45" s="4">
         <f>C44/HighResHz</f>
-        <v>2.6666673024495442E-9</v>
+        <v>3.4299666666666668E-4</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>11</v>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="C46" s="4">
         <f>C45+C24</f>
-        <v>4.0010000026666672</v>
+        <v>5.3453429966666661</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>11</v>

</xml_diff>